<commit_message>
Ready for final reactive testing
</commit_message>
<xml_diff>
--- a/Diversification-Tool-3.xlsx
+++ b/Diversification-Tool-3.xlsx
@@ -517,8 +517,8 @@
   </sheetPr>
   <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P18" activeCellId="0" sqref="P18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H5" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -760,7 +760,7 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="16" t="n">
-        <v>117.08</v>
+        <v>72.56</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>15</v>
@@ -825,7 +825,7 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="16" t="n">
-        <v>6</v>
+        <v>-10</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>19</v>
@@ -890,7 +890,7 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="16" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>21</v>
@@ -932,7 +932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -955,7 +955,7 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>24</v>
@@ -991,8 +991,7 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="16" t="n">
-        <f aca="false">B12+D12-E12</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>22</v>
@@ -1057,7 +1056,7 @@
       </c>
       <c r="P14" s="5" t="n">
         <f aca="false">J8+J9*1/4*(Q7+R7+S7+T7)+J10*1/4*(Q8+R8+S8+T8)+J12*1/4*(Q10+R10+S10+T10) + J11*1/4*(Q9+R9+S9+T9)</f>
-        <v>192.08</v>
+        <v>172.56</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="V14" s="8"/>
@@ -1246,7 +1245,7 @@
       <c r="K20" s="27"/>
       <c r="L20" s="28" t="n">
         <f aca="false">P14-P13*P25</f>
-        <v>182.826875</v>
+        <v>111.856875</v>
       </c>
       <c r="M20" s="29"/>
       <c r="T20" s="1" t="s">
@@ -1273,7 +1272,7 @@
       <c r="K21" s="29"/>
       <c r="L21" s="29" t="n">
         <f aca="false">P14/SQRT(P25)</f>
-        <v>5.28307714617037</v>
+        <v>1.85303502220371</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>36</v>
@@ -1319,7 +1318,7 @@
       </c>
       <c r="P25" s="5" t="n">
         <f aca="false">J9^2*U18+J10^2*U19+J11^2*U20+J12^2*U21+2*J9*J10*U23+2*J9*J12*U24+2*J10*J12*U25 + 2*J11*J12*U26+2*J9*J11*U27+2*J10*J11*U28</f>
-        <v>1321.875</v>
+        <v>8671.875</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>41</v>
@@ -1383,7 +1382,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -1406,7 +1405,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
market maker seems okay on 1017
</commit_message>
<xml_diff>
--- a/Diversification-Tool-3.xlsx
+++ b/Diversification-Tool-3.xlsx
@@ -518,7 +518,7 @@
   <dimension ref="A1:AA28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H5" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -737,7 +737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -760,7 +760,7 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="16" t="n">
-        <v>89.91</v>
+        <v>0.04</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>15</v>
@@ -802,7 +802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -825,7 +825,7 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="16" t="n">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>19</v>
@@ -867,7 +867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -890,7 +890,7 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>21</v>
@@ -955,7 +955,7 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="16" t="n">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>24</v>
@@ -968,7 +968,7 @@
       <c r="Y11" s="20"/>
       <c r="Z11" s="20"/>
     </row>
-    <row r="12" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -991,7 +991,7 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="16" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>22</v>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="P14" s="5" t="n">
         <f aca="false">J8+J9*1/4*(Q7+R7+S7+T7)+J10*1/4*(Q8+R8+S8+T8)+J12*1/4*(Q10+R10+S10+T10) + J11*1/4*(Q9+R9+S9+T9)</f>
-        <v>119.91</v>
+        <v>95.04</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="V14" s="8"/>
@@ -1181,6 +1181,9 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
+      <c r="N18" s="1" t="n">
+        <v>27.8525</v>
+      </c>
       <c r="T18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1221,6 +1224,10 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="M19" s="2"/>
+      <c r="O19" s="1" t="n">
+        <f aca="false">L20-N18</f>
+        <v>-5.00000000000001</v>
+      </c>
       <c r="T19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1245,7 +1252,7 @@
       <c r="K20" s="27"/>
       <c r="L20" s="28" t="n">
         <f aca="false">P14-P13*P25</f>
-        <v>117.8975</v>
+        <v>22.8525</v>
       </c>
       <c r="M20" s="29"/>
       <c r="T20" s="1" t="s">
@@ -1272,7 +1279,7 @@
       <c r="K21" s="29"/>
       <c r="L21" s="29" t="n">
         <f aca="false">P14/SQRT(P25)</f>
-        <v>7.07190598501349</v>
+        <v>0.935889224214063</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>36</v>
@@ -1318,7 +1325,7 @@
       </c>
       <c r="P25" s="5" t="n">
         <f aca="false">J9^2*U18+J10^2*U19+J11^2*U20+J12^2*U21+2*J9*J10*U23+2*J9*J12*U24+2*J10*J12*U25 + 2*J11*J12*U26+2*J9*J11*U27+2*J10*J11*U28</f>
-        <v>287.5</v>
+        <v>10312.5</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>41</v>

</xml_diff>